<commit_message>
Update document management process measures
</commit_message>
<xml_diff>
--- a/Docs/Processes/Documents Measures.xlsx
+++ b/Docs/Processes/Documents Measures.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
   <si>
     <t>Document Name</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Processes List</t>
+  </si>
+  <si>
+    <t>V0.2</t>
   </si>
 </sst>
 </file>
@@ -269,34 +272,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -307,6 +292,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -316,13 +302,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,12 +629,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
@@ -639,7 +644,7 @@
     <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5.140625" bestFit="1" customWidth="1"/>
@@ -650,250 +655,256 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="10" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="11"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="7"/>
-      <c r="P2" s="5"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="20"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="6" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="6" t="s">
+      <c r="F3" s="19"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="6" t="s">
+      <c r="I3" s="19"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="7"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="6" t="s">
+      <c r="L3" s="19"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="O3" s="7"/>
-      <c r="P3" s="5"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="20"/>
     </row>
     <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="N4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="O4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="P4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="20"/>
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="16"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="16" t="s">
+      <c r="B6" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="12">
+      <c r="G6" s="7">
+        <v>41328</v>
+      </c>
+      <c r="H6" s="6">
         <v>1</v>
       </c>
-      <c r="F6" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="13">
-        <v>41328</v>
-      </c>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
+      <c r="I6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="7">
+        <v>41332</v>
+      </c>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="15" t="s">
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="6">
         <f>SUM(E6:E10)</f>
         <v>1</v>
       </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12">
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6">
         <f>SUM(H6:H10)</f>
-        <v>0</v>
-      </c>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12">
+        <v>1</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6">
         <f>SUM(K6:K10)</f>
         <v>0</v>
       </c>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12">
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6">
         <f>SUM(N6:N10)</f>
         <v>0</v>
       </c>
-      <c r="O11" s="14"/>
-      <c r="P11" s="14"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
@@ -928,141 +939,141 @@
       <c r="N13" s="1"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="12">
+      <c r="D14" s="14"/>
+      <c r="E14" s="6">
         <v>1</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="13">
+      <c r="G14" s="7">
         <v>41328</v>
       </c>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="14"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14"/>
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="14"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="15" t="s">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E19" s="6">
         <f>SUM(E14:E18)</f>
         <v>1</v>
       </c>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12">
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6">
         <f>SUM(H14:H18)</f>
         <v>0</v>
       </c>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12">
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6">
         <f>SUM(K14:K18)</f>
         <v>0</v>
       </c>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12">
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6">
         <f>SUM(N14:N18)</f>
         <v>0</v>
       </c>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="10" t="s">
         <v>9</v>
       </c>
       <c r="E23">
@@ -1071,7 +1082,7 @@
       </c>
       <c r="H23">
         <f>SUM(H11,H19)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23">
         <f>SUM(K11,K19)</f>
@@ -1084,6 +1095,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A5:P5"/>
+    <mergeCell ref="F2:P2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="N3:P3"/>
     <mergeCell ref="A14:A19"/>
     <mergeCell ref="B14:B19"/>
     <mergeCell ref="C14:C19"/>
@@ -1092,12 +1109,6 @@
     <mergeCell ref="B6:B11"/>
     <mergeCell ref="C6:C11"/>
     <mergeCell ref="D6:D10"/>
-    <mergeCell ref="A5:P5"/>
-    <mergeCell ref="F2:P2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="N3:P3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>